<commit_message>
fix probe mapping to include probe A32 to adapter A32 (!!!)
</commit_message>
<xml_diff>
--- a/Neuronexus/Adapters/A32_Neuronexus_to_RHD2132_Mapping.xlsx
+++ b/Neuronexus/Adapters/A32_Neuronexus_to_RHD2132_Mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\silicon-probes\Neuronexus\Adapters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9DB70A-8949-4341-81F5-D7BE638BA538}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF996E51-52A9-4995-9EFB-1758F2AB6BF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7140" xr2:uid="{20D92B7F-9C7A-4719-83F9-24D0A88C73EE}"/>
   </bookViews>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Intan</t>
   </si>
   <si>
-    <t>A32</t>
+    <t>A32 (Adapter Side)</t>
+  </si>
+  <si>
+    <t>A32 (Probe Side)</t>
   </si>
 </sst>
 </file>
@@ -382,280 +385,384 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBEE6E6F-5114-4D82-84E8-E5C0B9EE5E28}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C27">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="C31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B33">
+  <sortState ref="A2:C33">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>